<commit_message>
Generate model outputs and forecasts
</commit_message>
<xml_diff>
--- a/model/datasets/Dengue_ARMM.xlsx
+++ b/model/datasets/Dengue_ARMM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cirrolytix\Hackathon\NASA Space Challenge 2019\01_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Documents\GitHub\nasa_hack\model\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C75F88-0521-4BAD-B048-EF8C20AF044E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D4FA4B-2DD5-477B-BA32-3629DC2FB354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{86AA2B33-C2F3-49C5-BF51-D8BC25F33613}"/>
   </bookViews>
@@ -45,13 +45,13 @@
     <t>GTrend_Dengue</t>
   </si>
   <si>
-    <t>Gtrend_Dengue_Sym</t>
-  </si>
-  <si>
     <t>Reg_Ave_Temp_ARMM</t>
   </si>
   <si>
     <t>Reg_Ave_Rainfall_ARMM</t>
+  </si>
+  <si>
+    <t>GTrend_Dengue_Sym</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,16 +432,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>